<commit_message>
Se avanza en el sistema de usuarios
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\U de A\semestres\semestre_2\materias\informatica_II\proyecto_final\Proyecto_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24030459-0ECC-4C2A-ACAA-FD937EFB63E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9BB1D4-E286-4B92-801E-2C652FFB5E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="15" windowWidth="20640" windowHeight="11160" xr2:uid="{3C2D6A2D-6351-4EE6-8208-3772497A4F05}"/>
   </bookViews>
@@ -276,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -327,19 +327,22 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E58666-0F6C-427E-8F85-4022D272E9E5}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -692,31 +695,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26" t="s">
         <v>23</v>
       </c>
       <c r="S1" s="24" t="s">
@@ -725,8 +728,8 @@
       <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
@@ -766,10 +769,10 @@
       <c r="O2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="23"/>
+      <c r="Q2" s="26"/>
       <c r="S2" s="2" t="s">
         <v>18</v>
       </c>
@@ -833,7 +836,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="11"/>
+      <c r="Q4" s="27"/>
       <c r="S4" s="2" t="s">
         <v>29</v>
       </c>
@@ -901,10 +904,10 @@
       <c r="O6" s="2"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="11"/>
-      <c r="S6" s="22" t="s">
+      <c r="S6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="T6" s="22"/>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18">

</xml_diff>

<commit_message>
Se agg la funcionalidad de crear una cuenta
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\U de A\semestres\semestre_2\materias\informatica_II\proyecto_final\Proyecto_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9BB1D4-E286-4B92-801E-2C652FFB5E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0820CB0-4D67-406B-8724-883D878626A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="15" windowWidth="20640" windowHeight="11160" xr2:uid="{3C2D6A2D-6351-4EE6-8208-3772497A4F05}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="36">
   <si>
     <t>#</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Multiventana</t>
   </si>
   <si>
-    <t>Enemigos</t>
-  </si>
-  <si>
     <t>Pruebas</t>
   </si>
   <si>
@@ -139,13 +136,19 @@
   </si>
   <si>
     <t>DOMINGO</t>
+  </si>
+  <si>
+    <t>Enemigos (Autos - Obstaculos)</t>
+  </si>
+  <si>
+    <t>Crater en la carretera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +172,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -276,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -331,6 +340,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,7 +355,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -663,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E58666-0F6C-427E-8F85-4022D272E9E5}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -695,41 +717,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="25"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="27"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
@@ -749,7 +771,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>5</v>
@@ -770,14 +792,14 @@
         <v>10</v>
       </c>
       <c r="P2" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="26"/>
+        <v>33</v>
+      </c>
+      <c r="Q2" s="28"/>
       <c r="S2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -785,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -805,10 +827,10 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="21"/>
       <c r="S3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -820,10 +842,10 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
@@ -836,16 +858,16 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="27"/>
+      <c r="Q4" s="24"/>
       <c r="S4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18">
+      <c r="A5" s="23">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -856,13 +878,13 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -870,23 +892,23 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="11"/>
+      <c r="Q5" s="30"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18">
+      <c r="A6" s="23">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -895,22 +917,22 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="11"/>
-      <c r="S6" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="T6" s="23"/>
+      <c r="Q6" s="31"/>
+      <c r="S6" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="23">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -920,11 +942,11 @@
       <c r="D7" s="2"/>
       <c r="E7" s="1"/>
       <c r="F7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="2"/>
@@ -932,31 +954,31 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O7" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="11"/>
+      <c r="Q7" s="24"/>
       <c r="S7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="T7" s="12"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18">
+      <c r="A8" s="23">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -964,25 +986,27 @@
       <c r="I8" s="18"/>
       <c r="J8" s="2"/>
       <c r="K8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="11"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="12"/>
+      <c r="Q8" s="24"/>
+      <c r="S8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="13"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="23">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="5"/>
@@ -990,32 +1014,32 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="2"/>
       <c r="K9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="11"/>
-      <c r="S9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="T9" s="13"/>
+      <c r="S9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="T9" s="14"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="23">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="5"/>
@@ -1027,26 +1051,28 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N10" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="11"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="13"/>
+      <c r="S10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T10" s="15"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="23">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1056,132 +1082,147 @@
       <c r="H11" s="2"/>
       <c r="I11" s="18"/>
       <c r="J11" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="11"/>
-      <c r="S11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T11" s="14"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="23">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="P12" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="3"/>
       <c r="Q12" s="11"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="14"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="23">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="5"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="18"/>
-      <c r="J13" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="M13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="19" t="s">
+        <v>27</v>
+      </c>
       <c r="P13" s="1"/>
       <c r="Q13" s="11"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="14"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="23">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>15</v>
+      <c r="B14" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="19" t="s">
-        <v>28</v>
+      <c r="D14" s="2"/>
+      <c r="E14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="P14" s="19" t="s">
-        <v>28</v>
-      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="1"/>
       <c r="Q14" s="11"/>
-      <c r="S14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T14" s="15"/>
+      <c r="S14" s="29"/>
+      <c r="T14" s="29"/>
+    </row>
+    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Se finaliza el planteamiento del multijugador. Ahora, pruebas
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\U de A\semestres\semestre_2\materias\informatica_II\proyecto_final\Proyecto_Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Google Drive\Semestre II\Informatica II\Info Teoria\Proyecto_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0820CB0-4D67-406B-8724-883D878626A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E91616D-519B-4B03-A5ED-7BBB649F5BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="15" windowWidth="20640" windowHeight="11160" xr2:uid="{3C2D6A2D-6351-4EE6-8208-3772497A4F05}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C2D6A2D-6351-4EE6-8208-3772497A4F05}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,12 +172,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFFC000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -285,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -309,9 +303,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -333,14 +324,15 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -353,16 +345,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E58666-0F6C-427E-8F85-4022D272E9E5}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -770,7 +752,7 @@
       <c r="H2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="17" t="s">
         <v>33</v>
       </c>
       <c r="J2" s="10" t="s">
@@ -791,7 +773,7 @@
       <c r="O2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="20" t="s">
         <v>33</v>
       </c>
       <c r="Q2" s="28"/>
@@ -803,13 +785,13 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="10"/>
@@ -817,7 +799,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="18"/>
+      <c r="I3" s="17"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
@@ -825,32 +807,32 @@
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="21"/>
+      <c r="Q3" s="13"/>
       <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18">
+      <c r="A4" s="17">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="18"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -858,16 +840,16 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="24"/>
+      <c r="Q4" s="13"/>
       <c r="S4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="21">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
@@ -877,13 +859,13 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="G5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>16</v>
       </c>
       <c r="K5" s="2"/>
@@ -892,47 +874,47 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="30"/>
+      <c r="Q5" s="13"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="21">
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="C6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="18"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="2"/>
-      <c r="N6" s="19" t="s">
+      <c r="N6" s="18" t="s">
         <v>27</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="31"/>
+      <c r="Q6" s="13"/>
       <c r="S6" s="25" t="s">
         <v>20</v>
       </c>
       <c r="T6" s="25"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="21">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -948,7 +930,7 @@
       <c r="H7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -960,14 +942,14 @@
         <v>19</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="24"/>
+      <c r="Q7" s="13"/>
       <c r="S7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="12"/>
+      <c r="T7" s="11"/>
     </row>
     <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23">
+      <c r="A8" s="21">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -983,7 +965,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="18"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="2"/>
       <c r="K8" s="9" t="s">
         <v>19</v>
@@ -995,14 +977,14 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="13"/>
       <c r="S8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T8" s="13"/>
+      <c r="T8" s="12"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="23">
+      <c r="A9" s="21">
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -1016,7 +998,7 @@
       <c r="H9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="2"/>
       <c r="K9" s="9" t="s">
         <v>19</v>
@@ -1028,14 +1010,14 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="11"/>
+      <c r="Q9" s="13"/>
       <c r="S9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="14"/>
+      <c r="T9" s="13"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="21">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1047,28 +1029,28 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="18"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N10" s="17" t="s">
+      <c r="L10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="16" t="s">
         <v>16</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="11"/>
+      <c r="Q10" s="13"/>
       <c r="S10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T10" s="15"/>
+      <c r="T10" s="14"/>
     </row>
     <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="21">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1080,26 +1062,26 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="17" t="s">
+      <c r="I11" s="17"/>
+      <c r="J11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="17" t="s">
+      <c r="M11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="11"/>
+      <c r="Q11" s="13"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="21">
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1111,7 +1093,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="32"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1122,7 +1104,7 @@
       <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="21">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1134,26 +1116,26 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="18"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
-      <c r="M13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" s="19" t="s">
+      <c r="M13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" s="18" t="s">
         <v>27</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="11"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
+      <c r="Q13" s="13"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="22"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="23">
+      <c r="A14" s="21">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1169,11 +1151,11 @@
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="K14" s="17" t="s">
+      <c r="I14" s="17"/>
+      <c r="J14" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>16</v>
       </c>
       <c r="L14" s="2"/>
@@ -1181,12 +1163,12 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="11"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
+      <c r="Q14" s="13"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="A15" s="21">
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -1195,34 +1177,34 @@
       <c r="C15" s="2"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="19" t="s">
+      <c r="H15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15" s="19" t="s">
+      <c r="K15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="N15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="P15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q15" s="31"/>
+      <c r="N15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
ULTIMO COMMIT DE MIGUEL :)
</commit_message>
<xml_diff>
--- a/cronograma.xlsx
+++ b/cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\Google Drive\Semestre II\Informatica II\Info Teoria\Proyecto_Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\U de A\semestres\semestre_2\materias\informatica_II\proyecto_final\Proyecto_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E91616D-519B-4B03-A5ED-7BBB649F5BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E58961-1B10-4DA1-A660-C1E407347F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C2D6A2D-6351-4EE6-8208-3772497A4F05}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{3C2D6A2D-6351-4EE6-8208-3772497A4F05}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -329,9 +329,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -345,6 +342,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,7 +670,7 @@
   <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -699,41 +699,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28" t="s">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28" t="s">
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="27"/>
+      <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
@@ -776,7 +776,7 @@
       <c r="P2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="28"/>
+      <c r="Q2" s="27"/>
       <c r="S2" s="2" t="s">
         <v>17</v>
       </c>
@@ -807,7 +807,7 @@
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="13"/>
+      <c r="Q3" s="14"/>
       <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="13"/>
+      <c r="Q4" s="14"/>
       <c r="S4" s="2" t="s">
         <v>28</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="13"/>
+      <c r="Q5" s="14"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
@@ -907,11 +907,11 @@
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="13"/>
-      <c r="S6" s="25" t="s">
+      <c r="Q6" s="14"/>
+      <c r="S6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="25"/>
+      <c r="T6" s="24"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
@@ -942,7 +942,7 @@
         <v>19</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="Q7" s="13"/>
+      <c r="Q7" s="14"/>
       <c r="S7" s="1" t="s">
         <v>21</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="13"/>
+      <c r="Q8" s="14"/>
       <c r="S8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1010,7 +1010,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="13"/>
+      <c r="Q9" s="14"/>
       <c r="S9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="13"/>
+      <c r="Q10" s="14"/>
       <c r="S10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="1"/>
-      <c r="Q11" s="13"/>
+      <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
@@ -1093,7 +1093,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="24"/>
+      <c r="I12" s="23"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -1130,7 +1130,7 @@
         <v>27</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="Q13" s="13"/>
+      <c r="Q13" s="14"/>
       <c r="S13" s="22"/>
       <c r="T13" s="22"/>
     </row>
@@ -1163,7 +1163,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="1"/>
-      <c r="Q14" s="13"/>
+      <c r="Q14" s="14"/>
       <c r="S14" s="22"/>
       <c r="T14" s="22"/>
     </row>
@@ -1204,7 +1204,7 @@
       <c r="P15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="Q15" s="23"/>
+      <c r="Q15" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>